<commit_message>
UFCE survey items refined
</commit_message>
<xml_diff>
--- a/BackEnd/LogData/output.xlsx
+++ b/BackEnd/LogData/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>userId</t>
   </si>
@@ -43,16 +43,7 @@
     <t>newPred_DiCE</t>
   </si>
   <si>
-    <t>59d876bb3c4a4739ada2f1fa55f29e00</t>
-  </si>
-  <si>
-    <t>aaae9b60ec0941fa9cb80caa55ab0b78</t>
-  </si>
-  <si>
-    <t>d482a28165234201acf8b943bb0505a3</t>
-  </si>
-  <si>
-    <t>fa58848e0ec9443697f10ac607ee628c</t>
+    <t>09ee0a844a2345f393f2502ef4514d5b</t>
   </si>
 </sst>
 </file>
@@ -410,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,13 +447,13 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>29</v>
@@ -471,7 +462,7 @@
         <v>61</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -479,25 +470,25 @@
         <v>9</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E3">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="H3">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -508,28 +499,28 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="E4">
         <v>14</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H4">
-        <v>-21</v>
+        <v>14</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -540,198 +531,53 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>35</v>
       </c>
       <c r="H5">
-        <v>55</v>
+        <v>-21</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H6">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>37</v>
-      </c>
-      <c r="E7">
-        <v>24</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>47</v>
-      </c>
-      <c r="H7">
-        <v>14</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>29</v>
-      </c>
-      <c r="E8">
-        <v>61</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>29</v>
-      </c>
-      <c r="H8">
-        <v>61</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>29</v>
-      </c>
-      <c r="E9">
-        <v>61</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>29</v>
-      </c>
-      <c r="H9">
-        <v>61</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>32</v>
-      </c>
-      <c r="E10">
-        <v>29</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>47</v>
-      </c>
-      <c r="H10">
-        <v>14</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-      <c r="E11">
-        <v>17</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>35</v>
-      </c>
-      <c r="H11">
-        <v>-21</v>
-      </c>
-      <c r="I11">
         <v>1</v>
       </c>
     </row>

</xml_diff>